<commit_message>
updated and new plots
</commit_message>
<xml_diff>
--- a/LCK Summer 2020/EGR and MLR progression split.xlsx
+++ b/LCK Summer 2020/EGR and MLR progression split.xlsx
@@ -392,7 +392,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -562,7 +562,7 @@
         <v>3.4</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -576,7 +576,7 @@
         <v>14.6</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -590,7 +590,7 @@
         <v>13</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -604,7 +604,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -618,7 +618,7 @@
         <v>-20.8</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -632,7 +632,7 @@
         <v>-5.0999999999999996</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -646,7 +646,7 @@
         <v>4.8</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -660,7 +660,7 @@
         <v>-22.9</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -674,7 +674,7 @@
         <v>12.5</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -688,7 +688,7 @@
         <v>-4.4000000000000004</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>